<commit_message>
feature: added sound effect on projectile hit
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejkre\Desktop\CSE-4392-CSE-5392-Game-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356101DD-D4B3-1C47-90DF-AB74A68644BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96060D20-5B1D-436F-8CBB-399B3B8E5AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>File Name</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Notes/Other</t>
+  </si>
+  <si>
+    <t>87535__whiprealgood__splat</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Whiprealgood/sounds/87535/</t>
+  </si>
+  <si>
+    <t>Creative Commons License</t>
+  </si>
+  <si>
+    <t>Doesn't require attribution</t>
   </si>
 </sst>
 </file>
@@ -388,13 +400,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
@@ -402,7 +414,7 @@
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,6 +426,20 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature/sound effect on pickup
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejkre\Desktop\CSE-4392-CSE-5392-Game-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96060D20-5B1D-436F-8CBB-399B3B8E5AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090DD5B3-3000-4C9D-BC92-D3C19A4CE791}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>File Name</t>
   </si>
@@ -45,10 +45,13 @@
     <t>https://freesound.org/people/Whiprealgood/sounds/87535/</t>
   </si>
   <si>
-    <t>Creative Commons License</t>
-  </si>
-  <si>
     <t>Doesn't require attribution</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/suntemple/sounds/253172/</t>
+  </si>
+  <si>
+    <t>Creative Commons License 0</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -436,10 +439,21 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added a main menu with a start new game setup, WIP, but wanting to merge
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejkre\Desktop\CSE-4392-CSE-5392-Game-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96060D20-5B1D-436F-8CBB-399B3B8E5AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C0614B-BD0E-C44B-8149-213BD112C78D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>File Name</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Doesn't require attribution</t>
+  </si>
+  <si>
+    <t>https://www.fontspace.com/a-area-kilometer-50-font-f53888</t>
+  </si>
+  <si>
+    <t>Freeware</t>
+  </si>
+  <si>
+    <t>AreaKilometer50-ow3xB.ttf</t>
   </si>
 </sst>
 </file>
@@ -400,13 +409,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
@@ -414,7 +423,7 @@
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -440,6 +449,17 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implemented Raddish enemy with scaling difficulty and fixed player knockback issues
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1192B815-7F79-9F4A-91BE-E53E2021403D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29407A18-DD7B-6D48-8758-3D618BED5C34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25960" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>File Name</t>
   </si>
@@ -64,19 +64,56 @@
   </si>
   <si>
     <t>https://freesound.org/people/suntemple/sounds/253172/</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>night-city-street-game-background-tiles</t>
+  </si>
+  <si>
+    <t>https://elthen.itch.io/2d-pixel-art-vegetable-monsters-sprite-pack</t>
+  </si>
+  <si>
+    <t>Feel free to use the sprites in commercial/non-commercial projects!</t>
+  </si>
+  <si>
+    <t>https://free-game-assets.itch.io/night-city-street-2d-background-tiles</t>
+  </si>
+  <si>
+    <t>Pixel Art Vegetable Monsters Sprite Pack</t>
+  </si>
+  <si>
+    <t>no restrictions on use in commercial projects, as well as you can freely use each product in unlimited number of projects</t>
+  </si>
+  <si>
+    <t>Purchased by Bala</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF252525"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,8 +136,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,17 +454,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="131.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -482,6 +521,39 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: added big onion and poison gas generation that hurts the player while inside
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29407A18-DD7B-6D48-8758-3D618BED5C34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAA5235-76F4-0C43-B05C-B5AED3E3E991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25960" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>File Name</t>
   </si>
@@ -88,13 +88,25 @@
   </si>
   <si>
     <t>Purchased by Bala</t>
+  </si>
+  <si>
+    <t>explosion_01_strip13.png</t>
+  </si>
+  <si>
+    <t>"Bleed - http://remusprites.carbonmade.com/"</t>
+  </si>
+  <si>
+    <t>Creative Commons License 3</t>
+  </si>
+  <si>
+    <t>https://opengameart.org/content/simple-explosion-bleeds-game-art</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +124,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FF252525"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -136,10 +154,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,6 +540,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
feat: added spike enemy, I was going to do a tilemap, but this seems better
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAA5235-76F4-0C43-B05C-B5AED3E3E991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AA81BF-7E83-2045-8BE1-2D8C225B5C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25960" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>File Name</t>
   </si>
@@ -100,13 +100,25 @@
   </si>
   <si>
     <t>https://opengameart.org/content/simple-explosion-bleeds-game-art</t>
+  </si>
+  <si>
+    <t>spikes.png</t>
+  </si>
+  <si>
+    <t>https://opengameart.org/content/spikes-0</t>
+  </si>
+  <si>
+    <t>Public Domain CC0</t>
+  </si>
+  <si>
+    <t>No attribution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +145,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,16 +171,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,38 +579,55 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{158B8209-3EFC-D340-A6AA-4ACEB41B9E8C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: added health and gas mask pickups, high jump next
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AA81BF-7E83-2045-8BE1-2D8C225B5C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30075B9E-F377-8A44-98B9-A8479669308C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="39300" yWindow="1880" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>File Name</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>No attribution</t>
+  </si>
+  <si>
+    <t>pixel_icons_by_oceansdream.png</t>
+  </si>
+  <si>
+    <t>https://opengameart.org/content/various-inventory-24-pixel-icon-set</t>
+  </si>
+  <si>
+    <t>CC-BY 3.0, CC-BY-SA 3.0</t>
   </si>
 </sst>
 </file>
@@ -499,7 +508,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +537,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -542,7 +551,7 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -556,7 +565,7 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
@@ -567,7 +576,7 @@
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C5" t="s">
@@ -591,6 +600,17 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
@@ -600,7 +620,7 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -614,7 +634,7 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -627,6 +647,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{158B8209-3EFC-D340-A6AA-4ACEB41B9E8C}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{DC822095-EBDB-804D-B8FB-EB32A238C623}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{0F1BC7DC-B496-564D-B2BD-7263A0F98794}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: added high jump as well
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30075B9E-F377-8A44-98B9-A8479669308C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3630C1-6233-3D41-9CD5-5CE837117096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39300" yWindow="1880" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>File Name</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>CC-BY 3.0, CC-BY-SA 3.0</t>
+  </si>
+  <si>
+    <t>Energia.png</t>
+  </si>
+  <si>
+    <t>https://opengameart.org/content/energy-icon</t>
+  </si>
+  <si>
+    <t>CC-BY 4.0</t>
   </si>
 </sst>
 </file>
@@ -505,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,34 +622,45 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -652,8 +672,9 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: music trigger stuff, regening level0 and 1 now
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3630C1-6233-3D41-9CD5-5CE837117096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A58762-8043-9E4D-B05A-DE3B6D8BA894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39300" yWindow="1880" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="1340" yWindow="3120" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>File Name</t>
   </si>
@@ -130,6 +130,33 @@
   </si>
   <si>
     <t>CC-BY 4.0</t>
+  </si>
+  <si>
+    <t>the-epic-2-by-rafael-krux.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Epic 2  by Rafael Krux
+Link: https://filmmusic.io/song/5384-the-epic-2-
+License: http://creativecommons.org/licenses/by/4.0/
+ Music promoted on https://www.chosic.com/free-music/all/ </t>
+  </si>
+  <si>
+    <t>Requires Attribution</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25862/</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/26014/</t>
+  </si>
+  <si>
+    <t>makai-symphony-dragon-slayer.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dragon Slayer by Makai Symphony | https://soundcloud.com/makai-symphony
+Music promoted by https://www.chosic.com/free-music/all/
+Creative Commons Attribution-ShareAlike 3.0 Unported
+https://creativecommons.org/licenses/by-sa/3.0/</t>
   </si>
 </sst>
 </file>
@@ -193,12 +220,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,36 +661,64 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D17" t="s">
         <v>20</v>
       </c>
     </row>
@@ -672,8 +730,8 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
-    <hyperlink ref="B11" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B17" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
     <hyperlink ref="B8" r:id="rId9" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Added intro scene, renamed levels, updated tests, added music to scene
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A58762-8043-9E4D-B05A-DE3B6D8BA894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA87D71-4C74-BE46-895D-CA0F76225E6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="3120" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="2600" yWindow="3620" windowWidth="30980" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>File Name</t>
   </si>
@@ -157,13 +157,25 @@
 Music promoted by https://www.chosic.com/free-music/all/
 Creative Commons Attribution-ShareAlike 3.0 Unported
 https://creativecommons.org/licenses/by-sa/3.0/</t>
+  </si>
+  <si>
+    <t>John_Bartmann_-_14_-_Serial_Killer.mp3</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25100/</t>
+  </si>
+  <si>
+    <t>You are free to use this music in your projects with no required crediting. However, linking back is greatly appreciated. You can use the following text</t>
+  </si>
+  <si>
+    <t>Music: https://www.chosic.com/free-music/all/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -198,6 +210,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,6 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -546,11 +566,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
@@ -558,7 +578,7 @@
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -586,7 +606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -600,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -611,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="18">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -625,7 +645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -639,7 +659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -650,7 +670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -661,7 +681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="136">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -675,7 +695,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="136">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -689,12 +709,26 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="18">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="20">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -708,7 +742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="18">
       <c r="A17" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
feat: added post credits sequence, only visible IFF you beat the game
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA87D71-4C74-BE46-895D-CA0F76225E6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEF4B7F-FD67-5041-A77B-E0E27C42D723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="3620" windowWidth="30980" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>File Name</t>
   </si>
@@ -169,13 +169,22 @@
   </si>
   <si>
     <t>Music: https://www.chosic.com/free-music/all/</t>
+  </si>
+  <si>
+    <t>https://hildemuz.itch.io/banana-man</t>
+  </si>
+  <si>
+    <t>Banana Man</t>
+  </si>
+  <si>
+    <t>You can use it in your games freely if you download from here and provide information about me in your game.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,6 +226,12 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="19"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -239,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -249,6 +264,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -566,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -721,6 +737,17 @@
       </c>
       <c r="D11" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4">

</xml_diff>

<commit_message>
Updated branch to develop
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3630C1-6233-3D41-9CD5-5CE837117096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA87D71-4C74-BE46-895D-CA0F76225E6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39300" yWindow="1880" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="2600" yWindow="3620" windowWidth="30980" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>File Name</t>
   </si>
@@ -130,13 +130,52 @@
   </si>
   <si>
     <t>CC-BY 4.0</t>
+  </si>
+  <si>
+    <t>the-epic-2-by-rafael-krux.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Epic 2  by Rafael Krux
+Link: https://filmmusic.io/song/5384-the-epic-2-
+License: http://creativecommons.org/licenses/by/4.0/
+ Music promoted on https://www.chosic.com/free-music/all/ </t>
+  </si>
+  <si>
+    <t>Requires Attribution</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25862/</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/26014/</t>
+  </si>
+  <si>
+    <t>makai-symphony-dragon-slayer.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dragon Slayer by Makai Symphony | https://soundcloud.com/makai-symphony
+Music promoted by https://www.chosic.com/free-music/all/
+Creative Commons Attribution-ShareAlike 3.0 Unported
+https://creativecommons.org/licenses/by-sa/3.0/</t>
+  </si>
+  <si>
+    <t>John_Bartmann_-_14_-_Serial_Killer.mp3</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25100/</t>
+  </si>
+  <si>
+    <t>You are free to use this music in your projects with no required crediting. However, linking back is greatly appreciated. You can use the following text</t>
+  </si>
+  <si>
+    <t>Music: https://www.chosic.com/free-music/all/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +210,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,12 +239,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,13 +564,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
@@ -528,7 +578,7 @@
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -556,7 +606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -570,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -581,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="18">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -595,7 +645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -609,7 +659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -620,7 +670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -631,36 +681,78 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="136">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="136">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="16" spans="1:4" ht="20">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="17" spans="1:4" ht="18">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D17" t="s">
         <v>20</v>
       </c>
     </row>
@@ -672,8 +764,8 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
-    <hyperlink ref="B11" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B17" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
     <hyperlink ref="B8" r:id="rId9" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Music files and music credits
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejkre\Desktop\CSE-4392-CSE-5392-Game-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEF4B7F-FD67-5041-A77B-E0E27C42D723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B4929C-9FD2-47C2-9B74-745B073D048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="3620" windowWidth="30980" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="17325" yWindow="3960" windowWidth="38700" windowHeight="15345" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>File Name</t>
   </si>
@@ -178,13 +178,25 @@
   </si>
   <si>
     <t>You can use it in your games freely if you download from here and provide information about me in your game.</t>
+  </si>
+  <si>
+    <t>Komiku_-_02_-_Boss_4__Cobblestone_in_their_face.mp3</t>
+  </si>
+  <si>
+    <t>Loyalty_Freak_Music_-_04_-_Cant_Stop_My_Feet_.mp3</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25453/</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25495/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -580,21 +592,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
-    <col min="3" max="3" width="131.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="131.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -622,7 +634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -636,7 +648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -647,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -661,7 +673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -675,7 +687,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -686,7 +698,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -697,7 +709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="136">
+    <row r="9" spans="1:4" ht="126" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -711,7 +723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="136">
+    <row r="10" spans="1:4" ht="126" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -725,7 +737,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18">
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -739,7 +751,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24">
+    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -750,36 +762,58 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>20</v>
       </c>
     </row>
@@ -791,8 +825,8 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
-    <hyperlink ref="B16" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
-    <hyperlink ref="B17" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B17" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B18" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
     <hyperlink ref="B8" r:id="rId9" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Royalty free Punch and Jump. Updated Branch.
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isamhashmi/Desktop/CSE-5392/CSE-4392-CSE-5392-Game-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UTA proj\CSE-4392-CSE-5392-Game-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3630C1-6233-3D41-9CD5-5CE837117096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2377E3D8-ED7C-45AB-83CB-8C4F025A952F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39300" yWindow="1880" windowWidth="36140" windowHeight="12300" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>File Name</t>
   </si>
@@ -130,13 +130,85 @@
   </si>
   <si>
     <t>CC-BY 4.0</t>
+  </si>
+  <si>
+    <t>the-epic-2-by-rafael-krux.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Epic 2  by Rafael Krux
+Link: https://filmmusic.io/song/5384-the-epic-2-
+License: http://creativecommons.org/licenses/by/4.0/
+ Music promoted on https://www.chosic.com/free-music/all/ </t>
+  </si>
+  <si>
+    <t>Requires Attribution</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25862/</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/26014/</t>
+  </si>
+  <si>
+    <t>makai-symphony-dragon-slayer.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dragon Slayer by Makai Symphony | https://soundcloud.com/makai-symphony
+Music promoted by https://www.chosic.com/free-music/all/
+Creative Commons Attribution-ShareAlike 3.0 Unported
+https://creativecommons.org/licenses/by-sa/3.0/</t>
+  </si>
+  <si>
+    <t>John_Bartmann_-_14_-_Serial_Killer.mp3</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25100/</t>
+  </si>
+  <si>
+    <t>You are free to use this music in your projects with no required crediting. However, linking back is greatly appreciated. You can use the following text</t>
+  </si>
+  <si>
+    <t>Music: https://www.chosic.com/free-music/all/</t>
+  </si>
+  <si>
+    <t>https://hildemuz.itch.io/banana-man</t>
+  </si>
+  <si>
+    <t>Banana Man</t>
+  </si>
+  <si>
+    <t>You can use it in your games freely if you download from here and provide information about me in your game.</t>
+  </si>
+  <si>
+    <t>Komiku_-_02_-_Boss_4__Cobblestone_in_their_face.mp3</t>
+  </si>
+  <si>
+    <t>Loyalty_Freak_Music_-_04_-_Cant_Stop_My_Feet_.mp3</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25453/</t>
+  </si>
+  <si>
+    <t>https://www.chosic.com/download-audio/25495/</t>
+  </si>
+  <si>
+    <t>zapsplat_cartoon_frog_jump_26526.mp3</t>
+  </si>
+  <si>
+    <t>zapsplat_foley_clothing_body_hit_punch_72693.mp3</t>
+  </si>
+  <si>
+    <t>https://www.zapsplat.com/music/body-hit-punch-clothing/</t>
+  </si>
+  <si>
+    <t>https://www.zapsplat.com/music/cartoon-frog-jump/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +243,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="19"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,12 +278,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,21 +604,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
-    <col min="3" max="3" width="131.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="131.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -556,7 +646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -570,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -581,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -595,7 +685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -609,7 +699,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -620,7 +710,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -631,36 +721,133 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="19" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="20" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
@@ -672,9 +859,11 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
-    <hyperlink ref="B11" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B19" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B20" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
     <hyperlink ref="B8" r:id="rId9" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{0233DAF5-CD8B-4365-A917-56DB6771290D}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{A6C30DC3-6981-44A9-A8F0-4CA6F999F85A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Credits.gd and excel sheet
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejkre\Desktop\CSE-4392-CSE-5392-Game-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UTA proj\CSE-4392-CSE-5392-Game-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B4929C-9FD2-47C2-9B74-745B073D048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE51BB2-BAB3-41C4-9D0B-492EA238F8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17325" yWindow="3960" windowWidth="38700" windowHeight="15345" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
   <si>
     <t>File Name</t>
   </si>
@@ -190,6 +190,54 @@
   </si>
   <si>
     <t>https://www.chosic.com/download-audio/25495/</t>
+  </si>
+  <si>
+    <t>60013__qubodup__whoosh</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/qubodup/sounds/60013/</t>
+  </si>
+  <si>
+    <t>382735__schots__gun-shot</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/schots/sounds/382735/</t>
+  </si>
+  <si>
+    <t>588246__rkkaleikau__energy-weapon-laser</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/rkkaleikau/sounds/588246/</t>
+  </si>
+  <si>
+    <t>566435__merrick079__punch2</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Merrick079/sounds/566435/</t>
+  </si>
+  <si>
+    <t>232358__richerlandtv__heavy-impacts</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/RICHERlandTV/sounds/232358/</t>
+  </si>
+  <si>
+    <t>341247__sharesynth__jump01</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/sharesynth/sounds/341247/</t>
+  </si>
+  <si>
+    <t>561646__mattruthsound__hit-punch-cloth-pillow-bedding-004</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/MattRuthSound/sounds/561646/</t>
+  </si>
+  <si>
+    <t>433644__dersuperanton__game-over-sound</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/dersuperanton/sounds/433644/</t>
   </si>
 </sst>
 </file>
@@ -592,21 +640,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
-    <col min="3" max="3" width="131.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.125" customWidth="1"/>
+    <col min="3" max="3" width="131.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -634,7 +682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -648,7 +696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -659,7 +707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -673,7 +721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -687,7 +735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -698,7 +746,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -709,7 +757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -723,7 +771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -737,7 +785,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -751,7 +799,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="24" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -762,7 +810,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -773,7 +821,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -784,36 +832,124 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="25" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D26" t="s">
         <v>20</v>
       </c>
     </row>
@@ -825,9 +961,17 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
-    <hyperlink ref="B17" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
-    <hyperlink ref="B18" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
-    <hyperlink ref="B8" r:id="rId9" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
+    <hyperlink ref="B26" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B25" r:id="rId9" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{71B5FBD9-0672-4AD1-B137-7BA794C9848C}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{64F9546F-53D4-49E9-99BA-7270A0011A87}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{B20738AE-7C4A-4E25-B489-21E13A6AA961}"/>
+    <hyperlink ref="B18" r:id="rId13" xr:uid="{61E82F37-0BAC-451B-AE8D-FF8F571C73CF}"/>
+    <hyperlink ref="B21" r:id="rId14" xr:uid="{7AC148FD-2A89-4314-B695-24FAD2A7F138}"/>
+    <hyperlink ref="B20" r:id="rId15" xr:uid="{C6AA900A-11F3-4394-B409-FA7818BE1989}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{79DFFB4F-672F-41AB-8477-6E1A58190D27}"/>
+    <hyperlink ref="B22" r:id="rId17" xr:uid="{A16E74C8-EBD7-448F-8F73-299574A0F1EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rolling back Sources-And-Credits to merge with develop
</commit_message>
<xml_diff>
--- a/Sources-And-Credits.xlsx
+++ b/Sources-And-Credits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UTA proj\CSE-4392-CSE-5392-Game-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejkre\Desktop\CSE-4392-CSE-5392-Game-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE51BB2-BAB3-41C4-9D0B-492EA238F8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B4929C-9FD2-47C2-9B74-745B073D048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
+    <workbookView xWindow="17325" yWindow="3960" windowWidth="38700" windowHeight="15345" xr2:uid="{679C53AB-0F7C-FE43-A95C-F8139A669DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>File Name</t>
   </si>
@@ -190,54 +190,6 @@
   </si>
   <si>
     <t>https://www.chosic.com/download-audio/25495/</t>
-  </si>
-  <si>
-    <t>60013__qubodup__whoosh</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/qubodup/sounds/60013/</t>
-  </si>
-  <si>
-    <t>382735__schots__gun-shot</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/schots/sounds/382735/</t>
-  </si>
-  <si>
-    <t>588246__rkkaleikau__energy-weapon-laser</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/rkkaleikau/sounds/588246/</t>
-  </si>
-  <si>
-    <t>566435__merrick079__punch2</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/Merrick079/sounds/566435/</t>
-  </si>
-  <si>
-    <t>232358__richerlandtv__heavy-impacts</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/RICHERlandTV/sounds/232358/</t>
-  </si>
-  <si>
-    <t>341247__sharesynth__jump01</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/sharesynth/sounds/341247/</t>
-  </si>
-  <si>
-    <t>561646__mattruthsound__hit-punch-cloth-pillow-bedding-004</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/MattRuthSound/sounds/561646/</t>
-  </si>
-  <si>
-    <t>433644__dersuperanton__game-over-sound</t>
-  </si>
-  <si>
-    <t>https://freesound.org/people/dersuperanton/sounds/433644/</t>
   </si>
 </sst>
 </file>
@@ -640,21 +592,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C147F87D-D7E2-AE4C-B028-E7991D30E8F4}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
-    <col min="3" max="3" width="131.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.09765625" customWidth="1"/>
+    <col min="3" max="3" width="131.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -682,7 +634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -696,7 +648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -707,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -721,7 +673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -735,7 +687,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -746,7 +698,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -757,7 +709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="126" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -771,7 +723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="126" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -785,7 +737,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -799,7 +751,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -810,7 +762,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -821,7 +773,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -832,124 +784,36 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D18" t="s">
         <v>20</v>
       </c>
     </row>
@@ -961,17 +825,9 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{7B3EC371-75A7-C74C-8793-BDA46DA7E85A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{F735FB14-7404-4D41-AA23-992A71CEE02F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{34BA2C09-F15A-F047-B720-05BD17DC530F}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
-    <hyperlink ref="B26" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
-    <hyperlink ref="B25" r:id="rId9" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
-    <hyperlink ref="B15" r:id="rId10" xr:uid="{71B5FBD9-0672-4AD1-B137-7BA794C9848C}"/>
-    <hyperlink ref="B16" r:id="rId11" xr:uid="{64F9546F-53D4-49E9-99BA-7270A0011A87}"/>
-    <hyperlink ref="B17" r:id="rId12" xr:uid="{B20738AE-7C4A-4E25-B489-21E13A6AA961}"/>
-    <hyperlink ref="B18" r:id="rId13" xr:uid="{61E82F37-0BAC-451B-AE8D-FF8F571C73CF}"/>
-    <hyperlink ref="B21" r:id="rId14" xr:uid="{7AC148FD-2A89-4314-B695-24FAD2A7F138}"/>
-    <hyperlink ref="B20" r:id="rId15" xr:uid="{C6AA900A-11F3-4394-B409-FA7818BE1989}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{79DFFB4F-672F-41AB-8477-6E1A58190D27}"/>
-    <hyperlink ref="B22" r:id="rId17" xr:uid="{A16E74C8-EBD7-448F-8F73-299574A0F1EE}"/>
+    <hyperlink ref="B17" r:id="rId7" xr:uid="{269D3369-3F4D-C945-8B8B-92D876BED6FC}"/>
+    <hyperlink ref="B18" r:id="rId8" xr:uid="{3FE46C13-E369-EA4A-B6C7-E9C823627AE7}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{8FF512D7-C95B-8F41-AF18-58BDBEE5331F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>